<commit_message>
Format student name and address
</commit_message>
<xml_diff>
--- a/api/Templates/CSFunding 2017-18 Invoice Summary w Signature - Template.xlsx
+++ b/api/Templates/CSFunding 2017-18 Invoice Summary w Signature - Template.xlsx
@@ -21,6 +21,12 @@
   </si>
   <si>
     <t>Individual Student Information Sheet</t>
+  </si>
+  <si>
+    <t>Summary Information Sheet</t>
+  </si>
+  <si>
+    <t>For the Months of July 2017 to ${AsOfMonth} ${AsOfYear}</t>
   </si>
   <si>
     <r>
@@ -77,7 +83,73 @@
     <t>${SchoolDistrict.Name}</t>
   </si>
   <si>
+    <t>Invoice Prep Date:</t>
+  </si>
+  <si>
     <t>${Prepared}</t>
+  </si>
+  <si>
+    <t>Date Sent to SD:</t>
+  </si>
+  <si>
+    <t>${ToSchoolDistrict}</t>
+  </si>
+  <si>
+    <t>Date Sent to PDE:</t>
+  </si>
+  <si>
+    <t>${ToPDE}</t>
+  </si>
+  <si>
+    <t>JUL
+${FirstYear}</t>
+  </si>
+  <si>
+    <t>AUG
+${FirstYear}</t>
+  </si>
+  <si>
+    <t>SEP
+${FirstYear}</t>
+  </si>
+  <si>
+    <t>OCT
+${FirstYear}</t>
+  </si>
+  <si>
+    <t>NOV
+${FirstYear}</t>
+  </si>
+  <si>
+    <t>DEC
+${FirstYear}</t>
+  </si>
+  <si>
+    <t>JAN
+${SecondYear}</t>
+  </si>
+  <si>
+    <t>FEB
+${SecondYear}</t>
+  </si>
+  <si>
+    <t>MAR
+${SecondYear}</t>
+  </si>
+  <si>
+    <t>APR
+${SecondYear}</t>
+  </si>
+  <si>
+    <t>MAY
+${SecondYear}</t>
+  </si>
+  <si>
+    <t>JUNE
+${SecondYear}</t>
+  </si>
+  <si>
+    <t>Selected Expenditures per ADM</t>
   </si>
   <si>
     <t>Date of Birth</t>
@@ -86,7 +158,53 @@
     <t xml:space="preserve">CS Student </t>
   </si>
   <si>
+    <t>Amount
+Due</t>
+  </si>
+  <si>
+    <t>Nonspecial Education</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.July}</t>
+  </si>
+  <si>
     <t>Last Day</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.August}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.September}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.October}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.November}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.December}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.January}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.February}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.March}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.April}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.May}</t>
+  </si>
+  <si>
+    <t>${RegularEnrollments.June}</t>
+  </si>
+  <si>
+    <t>${SchoolDistrict.RegularRate}</t>
   </si>
   <si>
     <t>Date of IEP</t>
@@ -140,7 +258,7 @@
     <t>Prior</t>
   </si>
   <si>
-    <t>${Students[0].LastName}, ${Students[0].FirstName} ${Students[0].MiddleInitial}</t>
+    <t>${Students[0].FullName}</t>
   </si>
   <si>
     <t>${Students[0].DateOfBirth}</t>
@@ -152,374 +270,7 @@
     <t>${Students[0].PaSecuredID}</t>
   </si>
   <si>
-    <t>${Students[0].Street1} ${Students[0].Street2}</t>
-  </si>
-  <si>
-    <t>${Students[0].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Students[0].LastDay}</t>
-  </si>
-  <si>
-    <t>${Students[0].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Students[0].City}, ${Students[0].State} ${Students[0].ZipCode}</t>
-  </si>
-  <si>
-    <t>${Students[0].Grade}</t>
-  </si>
-  <si>
-    <t>${Students[0].FormerIep}</t>
-  </si>
-  <si>
-    <t>${Students[1].LastName}, ${Students[1].FirstName} ${Students[1].MiddleInitial}</t>
-  </si>
-  <si>
-    <t>${Students[1].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Students[1].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Students[1].PaSecuredID}</t>
-  </si>
-  <si>
-    <t>${Students[1].Street1} ${Students[1].Street2}</t>
-  </si>
-  <si>
-    <t>${Students[1].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Students[1].LastDay}</t>
-  </si>
-  <si>
-    <t>${Students[1].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Students[1].City}, ${Students[1].State} ${Students[1].ZipCode}</t>
-  </si>
-  <si>
-    <t>${Students[1].Grade}</t>
-  </si>
-  <si>
-    <t>${Students[1].FormerIep}</t>
-  </si>
-  <si>
-    <t>${Students[2].LastName}, ${Students[2].FirstName} ${Students[2].MiddleInitial}</t>
-  </si>
-  <si>
-    <t>${Students[2].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Students[2].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Students[2].PaSecuredID}</t>
-  </si>
-  <si>
-    <t>${Students[2].Street1} ${Students[2].Street2}</t>
-  </si>
-  <si>
-    <t>${Students[2].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Students[2].LastDay}</t>
-  </si>
-  <si>
-    <t>${Students[2].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Students[2].City}, ${Students[2].State} ${Students[2].ZipCode}</t>
-  </si>
-  <si>
-    <t>${Students[2].Grade}</t>
-  </si>
-  <si>
-    <t>${Students[2].FormerIep}</t>
-  </si>
-  <si>
-    <t>${Students[3].LastName}, ${Students[3].FirstName} ${Students[3].MiddleInitial}</t>
-  </si>
-  <si>
-    <t>${Students[3].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Students[3].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Students[3].PaSecuredID}</t>
-  </si>
-  <si>
-    <t>${Students[3].Street1} ${Students[3].Street2}</t>
-  </si>
-  <si>
-    <t>${Students[3].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Students[3].LastDay}</t>
-  </si>
-  <si>
-    <t>${Students[3].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>Summary Information Sheet</t>
-  </si>
-  <si>
-    <t>${Students[3].City}, ${Students[3].State} ${Students[3].ZipCode}</t>
-  </si>
-  <si>
-    <t>${Students[3].Grade}</t>
-  </si>
-  <si>
-    <t>${Students[3].FormerIep}</t>
-  </si>
-  <si>
-    <t>For the Months of July 2017 to ${AsOfMonth} ${AsOfYear}</t>
-  </si>
-  <si>
-    <t>${Students[4].LastName}, ${Students[4].FirstName} ${Students[4].MiddleInitial}</t>
-  </si>
-  <si>
-    <t>${Students[4].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Students[4].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Students[4].PaSecuredID}</t>
-  </si>
-  <si>
-    <t>${Students[4].Street1} ${Students[4].Street2}</t>
-  </si>
-  <si>
-    <t>${Students[4].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Students[4].LastDay}</t>
-  </si>
-  <si>
-    <t>${Students[4].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>Invoice Prep Date:</t>
-  </si>
-  <si>
-    <t>${Students[4].City}, ${Students[4].State} ${Students[4].ZipCode}</t>
-  </si>
-  <si>
-    <t>${Students[4].Grade}</t>
-  </si>
-  <si>
-    <t>${Students[4].FormerIep}</t>
-  </si>
-  <si>
-    <t>Date Sent to SD:</t>
-  </si>
-  <si>
-    <t>${ToSchoolDistrict}</t>
-  </si>
-  <si>
-    <t>Date Sent to PDE:</t>
-  </si>
-  <si>
-    <t>${ToPDE}</t>
-  </si>
-  <si>
-    <t>${Students[5].LastName}, ${Students[5].FirstName} ${Students[5].MiddleInitial}</t>
-  </si>
-  <si>
-    <t>${Students[5].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Students[5].CurrentIep}</t>
-  </si>
-  <si>
-    <t>JUL
-${FirstYear}</t>
-  </si>
-  <si>
-    <t>${Students[5].PaSecuredID}</t>
-  </si>
-  <si>
-    <t>${Students[5].Street1} ${Students[5].Street2}</t>
-  </si>
-  <si>
-    <t>${Students[5].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Students[5].LastDay}</t>
-  </si>
-  <si>
-    <t>${Students[5].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Students[5].City}, ${Students[5].State} ${Students[5].ZipCode}</t>
-  </si>
-  <si>
-    <t>${Students[5].Grade}</t>
-  </si>
-  <si>
-    <t>${Students[5].FormerIep}</t>
-  </si>
-  <si>
-    <t>AUG
-${FirstYear}</t>
-  </si>
-  <si>
-    <t>SEP
-${FirstYear}</t>
-  </si>
-  <si>
-    <t>OCT
-${FirstYear}</t>
-  </si>
-  <si>
-    <t>NOV
-${FirstYear}</t>
-  </si>
-  <si>
-    <t>DEC
-${FirstYear}</t>
-  </si>
-  <si>
-    <t>JAN
-${SecondYear}</t>
-  </si>
-  <si>
-    <t>FEB
-${SecondYear}</t>
-  </si>
-  <si>
-    <t>MAR
-${SecondYear}</t>
-  </si>
-  <si>
-    <t>APR
-${SecondYear}</t>
-  </si>
-  <si>
-    <t>MAY
-${SecondYear}</t>
-  </si>
-  <si>
-    <t>JUNE
-${SecondYear}</t>
-  </si>
-  <si>
-    <t>Selected Expenditures per ADM</t>
-  </si>
-  <si>
-    <t>${Students[6].LastName}, ${Students[6].FirstName} ${Students[6].MiddleInitial}</t>
-  </si>
-  <si>
-    <t>${Students[6].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Students[6].CurrentIep}</t>
-  </si>
-  <si>
-    <t>Amount
-Due</t>
-  </si>
-  <si>
-    <t>${Students[6].PaSecuredID}</t>
-  </si>
-  <si>
-    <t>${Students[6].Street1} ${Students[6].Street2}</t>
-  </si>
-  <si>
-    <t>${Students[6].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Students[6].LastDay}</t>
-  </si>
-  <si>
-    <t>${Students[6].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Students[6].City}, ${Students[6].State} ${Students[6].ZipCode}</t>
-  </si>
-  <si>
-    <t>${Students[6].Grade}</t>
-  </si>
-  <si>
-    <t>Nonspecial Education</t>
-  </si>
-  <si>
-    <t>${Students[6].FormerIep}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.July}</t>
-  </si>
-  <si>
-    <t>${Students[7].LastName}, ${Students[7].FirstName} ${Students[7].MiddleInitial}</t>
-  </si>
-  <si>
-    <t>${Students[7].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Students[7].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Students[7].PaSecuredID}</t>
-  </si>
-  <si>
-    <t>${Students[7].Street1} ${Students[7].Street2}</t>
-  </si>
-  <si>
-    <t>${Students[7].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Students[7].LastDay}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.August}</t>
-  </si>
-  <si>
-    <t>${Students[7].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.September}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.October}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.November}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.December}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.January}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.February}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.March}</t>
-  </si>
-  <si>
-    <t>${Students[7].City}, ${Students[7].State} ${Students[7].ZipCode}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.April}</t>
-  </si>
-  <si>
-    <t>${Students[8].Grade}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.May}</t>
-  </si>
-  <si>
-    <t>${RegularEnrollments.June}</t>
-  </si>
-  <si>
-    <t>${Students[7].FormerIep}</t>
-  </si>
-  <si>
-    <t>${SchoolDistrict.RegularRate}</t>
+    <t>${Students[0].Address1}</t>
   </si>
   <si>
     <t>Special Education</t>
@@ -564,10 +315,70 @@
     <t>${SchoolDistrict.SpecialRate}</t>
   </si>
   <si>
+    <t>${Students[0].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Students[0].LastDay}</t>
+  </si>
+  <si>
+    <t>${Students[0].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Students[0].Address2}</t>
+  </si>
+  <si>
+    <t>${Students[0].Grade}</t>
+  </si>
+  <si>
     <t>Total Amount Due Year to Date:</t>
   </si>
   <si>
+    <t>${Students[0].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Students[1].FullName}</t>
+  </si>
+  <si>
+    <t>${Students[1].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Students[1].CurrentIep}</t>
+  </si>
+  <si>
+    <t>${Students[1].PaSecuredID}</t>
+  </si>
+  <si>
+    <t>${Students[1].Address1}</t>
+  </si>
+  <si>
+    <t>${Students[1].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Students[1].LastDay}</t>
+  </si>
+  <si>
+    <t>${Students[1].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Students[1].Address2}</t>
+  </si>
+  <si>
+    <t>${Students[1].Grade}</t>
+  </si>
+  <si>
+    <t>${Students[1].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Students[2].FullName}</t>
+  </si>
+  <si>
     <t xml:space="preserve"> School District</t>
+  </si>
+  <si>
+    <t>${Students[2].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Students[2].CurrentIep}</t>
   </si>
   <si>
     <t>Check</t>
@@ -579,10 +390,43 @@
     <t xml:space="preserve"> Refund from</t>
   </si>
   <si>
+    <t>${Students[2].PaSecuredID}</t>
+  </si>
+  <si>
+    <t>${Students[2].Address1}</t>
+  </si>
+  <si>
     <t>Month</t>
   </si>
   <si>
+    <t>${Students[2].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Students[2].LastDay}</t>
+  </si>
+  <si>
+    <t>${Students[2].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Students[2].Address2}</t>
+  </si>
+  <si>
+    <t>${Students[2].Grade}</t>
+  </si>
+  <si>
+    <t>${Students[2].FormerIep}</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Direct Payment</t>
+  </si>
+  <si>
+    <t>${Students[3].FullName}</t>
+  </si>
+  <si>
+    <t>${Students[3].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Students[3].CurrentIep}</t>
   </si>
   <si>
     <t>Date</t>
@@ -594,25 +438,181 @@
     <t xml:space="preserve">  Charter School</t>
   </si>
   <si>
+    <t>${Students[3].PaSecuredID}</t>
+  </si>
+  <si>
+    <t>${Students[3].Address1}</t>
+  </si>
+  <si>
+    <t>${Students[3].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Students[3].LastDay}</t>
+  </si>
+  <si>
+    <t>${Students[3].IsSpecialEducation}</t>
+  </si>
+  <si>
     <t>July, ${FirstYear}</t>
+  </si>
+  <si>
+    <t>${Students[3].Address2}</t>
+  </si>
+  <si>
+    <t>${Students[3].Grade}</t>
+  </si>
+  <si>
+    <t>${Students[3].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Students[4].FullName}</t>
+  </si>
+  <si>
+    <t>${Students[4].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Students[4].CurrentIep}</t>
+  </si>
+  <si>
+    <t>${Students[4].PaSecuredID}</t>
+  </si>
+  <si>
+    <t>${Students[4].Address1}</t>
+  </si>
+  <si>
+    <t>${Students[4].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Students[4].LastDay}</t>
+  </si>
+  <si>
+    <t>${Students[4].IsSpecialEducation}</t>
   </si>
   <si>
     <t>${Transactions.July.Payment.CheckAmount}</t>
   </si>
   <si>
+    <t>${Students[4].Address2}</t>
+  </si>
+  <si>
+    <t>${Students[4].Grade}</t>
+  </si>
+  <si>
+    <t>${Students[4].FormerIep}</t>
+  </si>
+  <si>
     <t>${Transactions.July.Payment.CheckNumber}</t>
+  </si>
+  <si>
+    <t>${Students[5].FullName}</t>
+  </si>
+  <si>
+    <t>${Students[5].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Students[5].CurrentIep}</t>
   </si>
   <si>
     <t>${Transactions.July.Payment.Date}</t>
   </si>
   <si>
+    <t>${Students[5].PaSecuredID}</t>
+  </si>
+  <si>
+    <t>${Students[5].Address1}</t>
+  </si>
+  <si>
+    <t>${Students[5].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Students[5].LastDay}</t>
+  </si>
+  <si>
+    <t>${Students[5].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Students[5].Address2}</t>
+  </si>
+  <si>
+    <t>${Students[5].Grade}</t>
+  </si>
+  <si>
+    <t>${Students[5].FormerIep}</t>
+  </si>
+  <si>
     <t>${Transactions.July.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Students[6].FullName}</t>
+  </si>
+  <si>
+    <t>${Students[6].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Students[6].CurrentIep}</t>
   </si>
   <si>
     <t>${Transactions.July.Refund}</t>
   </si>
   <si>
+    <t>${Students[6].PaSecuredID}</t>
+  </si>
+  <si>
+    <t>${Students[6].Address1}</t>
+  </si>
+  <si>
+    <t>${Students[6].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Students[6].LastDay}</t>
+  </si>
+  <si>
+    <t>${Students[6].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Students[6].Address2}</t>
+  </si>
+  <si>
+    <t>${Students[6].Grade}</t>
+  </si>
+  <si>
+    <t>${Students[6].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Students[7].FullName}</t>
+  </si>
+  <si>
+    <t>${Students[7].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Students[7].CurrentIep}</t>
+  </si>
+  <si>
     <t>August</t>
+  </si>
+  <si>
+    <t>${Students[7].PaSecuredID}</t>
+  </si>
+  <si>
+    <t>${Students[7].Address1}</t>
+  </si>
+  <si>
+    <t>${Students[7].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Students[7].LastDay}</t>
+  </si>
+  <si>
+    <t>${Students[7].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Students[7].Address2}</t>
+  </si>
+  <si>
+    <t>${Students[8].Grade}</t>
+  </si>
+  <si>
+    <t>${Students[7].FormerIep}</t>
   </si>
   <si>
     <t>${Transactions.August.Payment.CheckAmount}</t>
@@ -899,12 +899,12 @@
       <name val="Arial"/>
     </font>
     <font>
-      <i/>
-      <sz val="8.0"/>
+      <sz val="9.0"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <i/>
+      <sz val="8.0"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -969,6 +969,20 @@
       <bottom/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -977,6 +991,17 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -1154,31 +1179,6 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -1329,10 +1329,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -1348,10 +1348,16 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1365,152 +1371,146 @@
     <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="4" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="8" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="21" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="21" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="23" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="23" fillId="0" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="24" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1650,8 +1650,8 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="2"/>
@@ -1661,17 +1661,17 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="9"/>
@@ -1712,7 +1712,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="1"/>
       <c r="H3" s="10" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -1742,7 +1742,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="1"/>
       <c r="H4" s="11" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -1764,21 +1764,21 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1792,26 +1792,26 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="12" t="s">
-        <v>4</v>
+      <c r="A6" s="13" t="s">
+        <v>6</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="62"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63" t="s">
-        <v>81</v>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="16" t="s">
-        <v>6</v>
+      <c r="N6" s="14"/>
+      <c r="O6" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1826,10 +1826,10 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="12" t="s">
-        <v>5</v>
+      <c r="A7" s="13" t="s">
+        <v>7</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1838,14 +1838,14 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="63" t="s">
-        <v>85</v>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="M7" s="1"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="16" t="s">
-        <v>86</v>
+      <c r="N7" s="14"/>
+      <c r="O7" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1860,8 +1860,8 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1870,14 +1870,14 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63" t="s">
-        <v>87</v>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="16" t="s">
-        <v>88</v>
+      <c r="N8" s="14"/>
+      <c r="O8" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -1949,47 +1949,47 @@
     </row>
     <row r="11" ht="39.0" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="64" t="s">
-        <v>92</v>
+      <c r="B11" s="22" t="s">
+        <v>14</v>
       </c>
-      <c r="C11" s="64" t="s">
-        <v>101</v>
+      <c r="C11" s="22" t="s">
+        <v>15</v>
       </c>
-      <c r="D11" s="64" t="s">
-        <v>102</v>
+      <c r="D11" s="22" t="s">
+        <v>16</v>
       </c>
-      <c r="E11" s="64" t="s">
-        <v>103</v>
+      <c r="E11" s="22" t="s">
+        <v>17</v>
       </c>
-      <c r="F11" s="64" t="s">
-        <v>104</v>
+      <c r="F11" s="22" t="s">
+        <v>18</v>
       </c>
-      <c r="G11" s="64" t="s">
-        <v>105</v>
+      <c r="G11" s="22" t="s">
+        <v>19</v>
       </c>
-      <c r="H11" s="64" t="s">
-        <v>106</v>
+      <c r="H11" s="22" t="s">
+        <v>20</v>
       </c>
-      <c r="I11" s="64" t="s">
-        <v>107</v>
+      <c r="I11" s="22" t="s">
+        <v>21</v>
       </c>
-      <c r="J11" s="64" t="s">
-        <v>108</v>
+      <c r="J11" s="22" t="s">
+        <v>22</v>
       </c>
-      <c r="K11" s="64" t="s">
-        <v>109</v>
+      <c r="K11" s="22" t="s">
+        <v>23</v>
       </c>
-      <c r="L11" s="64" t="s">
-        <v>110</v>
+      <c r="L11" s="22" t="s">
+        <v>24</v>
       </c>
-      <c r="M11" s="64" t="s">
-        <v>111</v>
+      <c r="M11" s="22" t="s">
+        <v>25</v>
       </c>
-      <c r="N11" s="65" t="s">
-        <v>112</v>
+      <c r="N11" s="24" t="s">
+        <v>26</v>
       </c>
-      <c r="O11" s="66" t="s">
-        <v>116</v>
+      <c r="O11" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -2004,49 +2004,49 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="67" t="s">
-        <v>124</v>
+      <c r="A12" s="27" t="s">
+        <v>30</v>
       </c>
-      <c r="B12" s="68" t="s">
-        <v>126</v>
+      <c r="B12" s="29" t="s">
+        <v>31</v>
       </c>
-      <c r="C12" s="68" t="s">
-        <v>134</v>
+      <c r="C12" s="29" t="s">
+        <v>33</v>
       </c>
-      <c r="D12" s="68" t="s">
-        <v>136</v>
+      <c r="D12" s="29" t="s">
+        <v>34</v>
       </c>
-      <c r="E12" s="68" t="s">
-        <v>137</v>
+      <c r="E12" s="29" t="s">
+        <v>35</v>
       </c>
-      <c r="F12" s="68" t="s">
-        <v>138</v>
+      <c r="F12" s="29" t="s">
+        <v>36</v>
       </c>
-      <c r="G12" s="68" t="s">
-        <v>139</v>
+      <c r="G12" s="29" t="s">
+        <v>37</v>
       </c>
-      <c r="H12" s="68" t="s">
-        <v>140</v>
+      <c r="H12" s="29" t="s">
+        <v>38</v>
       </c>
-      <c r="I12" s="68" t="s">
-        <v>141</v>
+      <c r="I12" s="29" t="s">
+        <v>39</v>
       </c>
-      <c r="J12" s="68" t="s">
-        <v>142</v>
+      <c r="J12" s="29" t="s">
+        <v>40</v>
       </c>
-      <c r="K12" s="68" t="s">
-        <v>144</v>
+      <c r="K12" s="29" t="s">
+        <v>41</v>
       </c>
-      <c r="L12" s="68" t="s">
-        <v>146</v>
+      <c r="L12" s="29" t="s">
+        <v>42</v>
       </c>
-      <c r="M12" s="68" t="s">
-        <v>147</v>
+      <c r="M12" s="29" t="s">
+        <v>43</v>
       </c>
-      <c r="N12" s="69" t="s">
-        <v>149</v>
+      <c r="N12" s="31" t="s">
+        <v>44</v>
       </c>
-      <c r="O12" s="70" t="str">
+      <c r="O12" s="54" t="str">
         <f t="shared" ref="O12:O13" si="1">ROUND(SUMIF(B12:M12,"&gt;0")*N12/12,2)</f>
         <v>#VALUE!</v>
       </c>
@@ -2063,49 +2063,49 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="67" t="s">
-        <v>150</v>
+      <c r="A13" s="27" t="s">
+        <v>67</v>
       </c>
-      <c r="B13" s="68" t="s">
-        <v>151</v>
+      <c r="B13" s="29" t="s">
+        <v>68</v>
       </c>
-      <c r="C13" s="68" t="s">
-        <v>152</v>
+      <c r="C13" s="29" t="s">
+        <v>69</v>
       </c>
-      <c r="D13" s="68" t="s">
-        <v>153</v>
+      <c r="D13" s="29" t="s">
+        <v>70</v>
       </c>
-      <c r="E13" s="68" t="s">
-        <v>154</v>
+      <c r="E13" s="29" t="s">
+        <v>71</v>
       </c>
-      <c r="F13" s="68" t="s">
-        <v>155</v>
+      <c r="F13" s="29" t="s">
+        <v>72</v>
       </c>
-      <c r="G13" s="68" t="s">
-        <v>156</v>
+      <c r="G13" s="29" t="s">
+        <v>73</v>
       </c>
-      <c r="H13" s="68" t="s">
-        <v>157</v>
+      <c r="H13" s="29" t="s">
+        <v>74</v>
       </c>
-      <c r="I13" s="68" t="s">
-        <v>158</v>
+      <c r="I13" s="29" t="s">
+        <v>75</v>
       </c>
-      <c r="J13" s="68" t="s">
-        <v>159</v>
+      <c r="J13" s="29" t="s">
+        <v>76</v>
       </c>
-      <c r="K13" s="68" t="s">
-        <v>160</v>
+      <c r="K13" s="29" t="s">
+        <v>77</v>
       </c>
-      <c r="L13" s="68" t="s">
-        <v>161</v>
+      <c r="L13" s="29" t="s">
+        <v>78</v>
       </c>
-      <c r="M13" s="68" t="s">
-        <v>162</v>
+      <c r="M13" s="29" t="s">
+        <v>79</v>
       </c>
-      <c r="N13" s="69" t="s">
-        <v>163</v>
+      <c r="N13" s="31" t="s">
+        <v>80</v>
       </c>
-      <c r="O13" s="70" t="str">
+      <c r="O13" s="54" t="str">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -2161,10 +2161,10 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="72" t="s">
-        <v>164</v>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="67" t="s">
+        <v>86</v>
       </c>
       <c r="O15" s="73" t="str">
         <f>SUM(O12:O13)</f>
@@ -2216,21 +2216,21 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="74" t="s">
-        <v>165</v>
+        <v>100</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="8" t="s">
-        <v>166</v>
+        <v>103</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>166</v>
+        <v>103</v>
       </c>
       <c r="I17" s="74" t="s">
-        <v>167</v>
+        <v>104</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="74" t="s">
-        <v>168</v>
+        <v>105</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -2252,25 +2252,25 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="75" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="D18" s="75"/>
       <c r="E18" s="76" t="s">
-        <v>170</v>
+        <v>115</v>
       </c>
-      <c r="F18" s="33"/>
+      <c r="F18" s="41"/>
       <c r="G18" s="8" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="I18" s="76" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="J18" s="77"/>
       <c r="K18" s="76" t="s">
-        <v>173</v>
+        <v>121</v>
       </c>
       <c r="L18" s="77"/>
       <c r="M18" s="77"/>
@@ -2292,26 +2292,26 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="78" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="D19" s="79"/>
       <c r="E19" s="80"/>
       <c r="F19" s="81" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="G19" s="82" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="H19" s="83" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="I19" s="84"/>
       <c r="J19" s="85" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="K19" s="84"/>
       <c r="L19" s="86" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="M19" s="87"/>
       <c r="N19" s="1"/>
@@ -2332,7 +2332,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="88"/>
@@ -2847,7 +2847,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="72" t="s">
+      <c r="N33" s="67" t="s">
         <v>246</v>
       </c>
       <c r="O33" s="109">
@@ -2908,7 +2908,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="N35" s="72" t="str">
+      <c r="N35" s="67" t="str">
         <f>IF(O15-O33&gt;=0,"Net Due to Charter School:","Net Due to School District:")</f>
         <v>#VALUE!</v>
       </c>
@@ -3113,7 +3113,7 @@
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="113" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K42" s="112"/>
       <c r="L42" s="112"/>
@@ -3144,7 +3144,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="114" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>251</v>
@@ -29999,7 +29999,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="3"/>
@@ -30090,7 +30090,7 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -30115,11 +30115,11 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="12" t="s">
-        <v>4</v>
+      <c r="B5" s="13" t="s">
+        <v>6</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="10"/>
@@ -30145,19 +30145,19 @@
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="12" t="s">
-        <v>5</v>
+      <c r="B6" s="13" t="s">
+        <v>7</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="16" t="s">
-        <v>6</v>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -30179,12 +30179,12 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -30205,23 +30205,23 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="18" t="s">
-        <v>7</v>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="20" t="s">
+        <v>27</v>
       </c>
-      <c r="G8" s="21" t="s">
-        <v>8</v>
+      <c r="G8" s="26" t="s">
+        <v>28</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23" t="s">
-        <v>9</v>
+      <c r="H8" s="28"/>
+      <c r="I8" s="30" t="s">
+        <v>32</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21" t="s">
-        <v>10</v>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -30241,25 +30241,25 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29" t="s">
-        <v>11</v>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37" t="s">
+        <v>46</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>12</v>
+      <c r="H9" s="38" t="s">
+        <v>47</v>
       </c>
-      <c r="I9" s="30" t="s">
-        <v>13</v>
+      <c r="I9" s="38" t="s">
+        <v>48</v>
       </c>
-      <c r="J9" s="29" t="s">
-        <v>14</v>
+      <c r="J9" s="37" t="s">
+        <v>49</v>
       </c>
-      <c r="K9" s="31" t="s">
-        <v>15</v>
+      <c r="K9" s="39" t="s">
+        <v>50</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -30279,33 +30279,33 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="24" t="s">
-        <v>16</v>
+      <c r="B10" s="32" t="s">
+        <v>51</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>17</v>
+      <c r="C10" s="33" t="s">
+        <v>52</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>18</v>
+      <c r="D10" s="33" t="s">
+        <v>53</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="21" t="s">
-        <v>19</v>
+      <c r="E10" s="35"/>
+      <c r="F10" s="26" t="s">
+        <v>54</v>
       </c>
-      <c r="G10" s="29" t="s">
-        <v>20</v>
+      <c r="G10" s="37" t="s">
+        <v>55</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>13</v>
+      <c r="H10" s="38" t="s">
+        <v>48</v>
       </c>
-      <c r="I10" s="32" t="s">
-        <v>21</v>
+      <c r="I10" s="40" t="s">
+        <v>56</v>
       </c>
-      <c r="J10" s="29" t="s">
-        <v>22</v>
+      <c r="J10" s="37" t="s">
+        <v>57</v>
       </c>
-      <c r="K10" s="21" t="s">
-        <v>10</v>
+      <c r="K10" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -30324,1135 +30324,1135 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="31" t="s">
-        <v>23</v>
+      <c r="A11" s="41"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="39" t="s">
+        <v>58</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="38" t="s">
-        <v>24</v>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46" t="s">
+        <v>59</v>
       </c>
-      <c r="J11" s="31" t="s">
-        <v>25</v>
+      <c r="J11" s="39" t="s">
+        <v>60</v>
       </c>
-      <c r="K11" s="31" t="s">
-        <v>26</v>
+      <c r="K11" s="39" t="s">
+        <v>61</v>
       </c>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="33"/>
-      <c r="Z11" s="33"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41" t="s">
-        <v>27</v>
+      <c r="A12" s="41"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49" t="s">
+        <v>62</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43" t="s">
-        <v>28</v>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51" t="s">
+        <v>63</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="43" t="s">
-        <v>29</v>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="51" t="s">
+        <v>64</v>
       </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
-      <c r="S12" s="33"/>
-      <c r="T12" s="33"/>
-      <c r="U12" s="33"/>
-      <c r="V12" s="33"/>
-      <c r="W12" s="33"/>
-      <c r="X12" s="33"/>
-      <c r="Y12" s="33"/>
-      <c r="Z12" s="33"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41"/>
+      <c r="Z12" s="41"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="46">
+      <c r="A13" s="41"/>
+      <c r="B13" s="55">
         <v>1.0</v>
       </c>
-      <c r="C13" s="47" t="s">
-        <v>30</v>
+      <c r="C13" s="56" t="s">
+        <v>65</v>
       </c>
-      <c r="D13" s="48" t="s">
-        <v>31</v>
+      <c r="D13" s="57" t="s">
+        <v>66</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="52" t="s">
-        <v>32</v>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61" t="s">
+        <v>81</v>
       </c>
-      <c r="I13" s="52" t="s">
-        <v>33</v>
+      <c r="I13" s="61" t="s">
+        <v>82</v>
       </c>
-      <c r="J13" s="53" t="s">
-        <v>34</v>
+      <c r="J13" s="62" t="s">
+        <v>83</v>
       </c>
-      <c r="K13" s="54"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="33"/>
-      <c r="S13" s="33"/>
-      <c r="T13" s="33"/>
-      <c r="U13" s="33"/>
-      <c r="V13" s="33"/>
-      <c r="W13" s="33"/>
-      <c r="X13" s="33"/>
-      <c r="Y13" s="33"/>
-      <c r="Z13" s="33"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="33"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="48" t="s">
-        <v>35</v>
+      <c r="A14" s="41"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="57" t="s">
+        <v>84</v>
       </c>
-      <c r="E14" s="49"/>
-      <c r="F14" s="56" t="s">
-        <v>36</v>
+      <c r="E14" s="58"/>
+      <c r="F14" s="66" t="s">
+        <v>85</v>
       </c>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="43" t="s">
-        <v>37</v>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="51" t="s">
+        <v>87</v>
       </c>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="33"/>
-      <c r="U14" s="33"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="33"/>
-      <c r="Y14" s="33"/>
-      <c r="Z14" s="33"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
-      <c r="X15" s="33"/>
-      <c r="Y15" s="33"/>
-      <c r="Z15" s="33"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="41"/>
+      <c r="W15" s="41"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="41"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41" t="s">
-        <v>38</v>
+      <c r="A16" s="41"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49" t="s">
+        <v>88</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43" t="s">
-        <v>39</v>
+      <c r="E16" s="50"/>
+      <c r="F16" s="51" t="s">
+        <v>89</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="43" t="s">
-        <v>40</v>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="51" t="s">
+        <v>90</v>
       </c>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
-      <c r="U16" s="33"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="33"/>
-      <c r="X16" s="33"/>
-      <c r="Y16" s="33"/>
-      <c r="Z16" s="33"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="41"/>
+      <c r="Z16" s="41"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="33"/>
-      <c r="B17" s="46">
+      <c r="A17" s="41"/>
+      <c r="B17" s="55">
         <f>B13+1</f>
         <v>2</v>
       </c>
-      <c r="C17" s="47" t="s">
-        <v>41</v>
+      <c r="C17" s="56" t="s">
+        <v>91</v>
       </c>
-      <c r="D17" s="48" t="s">
-        <v>42</v>
+      <c r="D17" s="57" t="s">
+        <v>92</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="52" t="s">
-        <v>43</v>
+      <c r="E17" s="58"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61" t="s">
+        <v>93</v>
       </c>
-      <c r="I17" s="52" t="s">
-        <v>44</v>
+      <c r="I17" s="61" t="s">
+        <v>94</v>
       </c>
-      <c r="J17" s="53" t="s">
-        <v>45</v>
+      <c r="J17" s="62" t="s">
+        <v>95</v>
       </c>
-      <c r="K17" s="54"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="33"/>
-      <c r="U17" s="33"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="33"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="33"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="41"/>
+      <c r="Z17" s="41"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="33"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="48" t="s">
-        <v>46</v>
+      <c r="A18" s="41"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="57" t="s">
+        <v>96</v>
       </c>
-      <c r="E18" s="49"/>
-      <c r="F18" s="56" t="s">
-        <v>47</v>
+      <c r="E18" s="58"/>
+      <c r="F18" s="66" t="s">
+        <v>97</v>
       </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="43" t="s">
-        <v>48</v>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="51" t="s">
+        <v>98</v>
       </c>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="33"/>
-      <c r="V18" s="33"/>
-      <c r="W18" s="33"/>
-      <c r="X18" s="33"/>
-      <c r="Y18" s="33"/>
-      <c r="Z18" s="33"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="41"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="33"/>
-      <c r="S19" s="33"/>
-      <c r="T19" s="33"/>
-      <c r="U19" s="33"/>
-      <c r="V19" s="33"/>
-      <c r="W19" s="33"/>
-      <c r="X19" s="33"/>
-      <c r="Y19" s="33"/>
-      <c r="Z19" s="33"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="41"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="41"/>
+      <c r="Z19" s="41"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="33"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41" t="s">
-        <v>49</v>
+      <c r="A20" s="41"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49" t="s">
+        <v>99</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43" t="s">
-        <v>50</v>
+      <c r="E20" s="50"/>
+      <c r="F20" s="51" t="s">
+        <v>101</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="43" t="s">
-        <v>51</v>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="51" t="s">
+        <v>102</v>
       </c>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="33"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="41"/>
+      <c r="Z20" s="41"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="33"/>
-      <c r="B21" s="46">
+      <c r="A21" s="41"/>
+      <c r="B21" s="55">
         <f>B17+1</f>
         <v>3</v>
       </c>
-      <c r="C21" s="47" t="s">
-        <v>52</v>
+      <c r="C21" s="56" t="s">
+        <v>106</v>
       </c>
-      <c r="D21" s="48" t="s">
-        <v>53</v>
+      <c r="D21" s="57" t="s">
+        <v>107</v>
       </c>
-      <c r="E21" s="49"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="52" t="s">
-        <v>54</v>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="61" t="s">
+        <v>109</v>
       </c>
-      <c r="I21" s="52" t="s">
-        <v>55</v>
+      <c r="I21" s="61" t="s">
+        <v>110</v>
       </c>
-      <c r="J21" s="53" t="s">
-        <v>56</v>
+      <c r="J21" s="62" t="s">
+        <v>111</v>
       </c>
-      <c r="K21" s="54"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="33"/>
-      <c r="V21" s="33"/>
-      <c r="W21" s="33"/>
-      <c r="X21" s="33"/>
-      <c r="Y21" s="33"/>
-      <c r="Z21" s="33"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41"/>
+      <c r="Z21" s="41"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="33"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="48" t="s">
-        <v>57</v>
+      <c r="A22" s="41"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="57" t="s">
+        <v>112</v>
       </c>
-      <c r="E22" s="49"/>
-      <c r="F22" s="56" t="s">
-        <v>58</v>
+      <c r="E22" s="58"/>
+      <c r="F22" s="66" t="s">
+        <v>113</v>
       </c>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="43" t="s">
-        <v>59</v>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="51" t="s">
+        <v>114</v>
       </c>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="33"/>
-      <c r="V22" s="33"/>
-      <c r="W22" s="33"/>
-      <c r="X22" s="33"/>
-      <c r="Y22" s="33"/>
-      <c r="Z22" s="33"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
+      <c r="V22" s="41"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="41"/>
+      <c r="Z22" s="41"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="33"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="33"/>
-      <c r="S23" s="33"/>
-      <c r="T23" s="33"/>
-      <c r="U23" s="33"/>
-      <c r="V23" s="33"/>
-      <c r="W23" s="33"/>
-      <c r="X23" s="33"/>
-      <c r="Y23" s="33"/>
-      <c r="Z23" s="33"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="41"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="41"/>
+      <c r="Z23" s="41"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="33"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="41" t="s">
-        <v>60</v>
+      <c r="A24" s="41"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49" t="s">
+        <v>116</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43" t="s">
-        <v>61</v>
+      <c r="E24" s="50"/>
+      <c r="F24" s="51" t="s">
+        <v>117</v>
       </c>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="43" t="s">
-        <v>62</v>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="51" t="s">
+        <v>118</v>
       </c>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="33"/>
-      <c r="W24" s="33"/>
-      <c r="X24" s="33"/>
-      <c r="Y24" s="33"/>
-      <c r="Z24" s="33"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
+      <c r="S24" s="41"/>
+      <c r="T24" s="41"/>
+      <c r="U24" s="41"/>
+      <c r="V24" s="41"/>
+      <c r="W24" s="41"/>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="41"/>
+      <c r="Z24" s="41"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="33"/>
-      <c r="B25" s="46">
+      <c r="A25" s="41"/>
+      <c r="B25" s="55">
         <f>B21+1</f>
         <v>4</v>
       </c>
-      <c r="C25" s="47" t="s">
-        <v>63</v>
+      <c r="C25" s="56" t="s">
+        <v>122</v>
       </c>
-      <c r="D25" s="48" t="s">
-        <v>64</v>
+      <c r="D25" s="57" t="s">
+        <v>123</v>
       </c>
-      <c r="E25" s="49"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="52" t="s">
-        <v>65</v>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="61" t="s">
+        <v>124</v>
       </c>
-      <c r="I25" s="52" t="s">
-        <v>66</v>
+      <c r="I25" s="61" t="s">
+        <v>125</v>
       </c>
-      <c r="J25" s="53" t="s">
-        <v>67</v>
+      <c r="J25" s="62" t="s">
+        <v>126</v>
       </c>
-      <c r="K25" s="54"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="33"/>
-      <c r="W25" s="33"/>
-      <c r="X25" s="33"/>
-      <c r="Y25" s="33"/>
-      <c r="Z25" s="33"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41"/>
+      <c r="U25" s="41"/>
+      <c r="V25" s="41"/>
+      <c r="W25" s="41"/>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="41"/>
+      <c r="Z25" s="41"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="33"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="48" t="s">
-        <v>69</v>
+      <c r="A26" s="41"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="57" t="s">
+        <v>128</v>
       </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="56" t="s">
-        <v>70</v>
+      <c r="E26" s="58"/>
+      <c r="F26" s="66" t="s">
+        <v>129</v>
       </c>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="43" t="s">
-        <v>71</v>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="51" t="s">
+        <v>130</v>
       </c>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="33"/>
-      <c r="S26" s="33"/>
-      <c r="T26" s="33"/>
-      <c r="U26" s="33"/>
-      <c r="V26" s="33"/>
-      <c r="W26" s="33"/>
-      <c r="X26" s="33"/>
-      <c r="Y26" s="33"/>
-      <c r="Z26" s="33"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
+      <c r="T26" s="41"/>
+      <c r="U26" s="41"/>
+      <c r="V26" s="41"/>
+      <c r="W26" s="41"/>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="41"/>
+      <c r="Z26" s="41"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="33"/>
-      <c r="X27" s="33"/>
-      <c r="Y27" s="33"/>
-      <c r="Z27" s="33"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41"/>
+      <c r="Z27" s="41"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="33"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="41" t="s">
-        <v>73</v>
+      <c r="A28" s="41"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49" t="s">
+        <v>131</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43" t="s">
-        <v>74</v>
+      <c r="E28" s="50"/>
+      <c r="F28" s="51" t="s">
+        <v>132</v>
       </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="43" t="s">
-        <v>75</v>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="51" t="s">
+        <v>133</v>
       </c>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="33"/>
-      <c r="S28" s="33"/>
-      <c r="T28" s="33"/>
-      <c r="U28" s="33"/>
-      <c r="V28" s="33"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="33"/>
-      <c r="Y28" s="33"/>
-      <c r="Z28" s="33"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="41"/>
+      <c r="V28" s="41"/>
+      <c r="W28" s="41"/>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="41"/>
+      <c r="Z28" s="41"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="33"/>
-      <c r="B29" s="46">
+      <c r="A29" s="41"/>
+      <c r="B29" s="55">
         <f>B25+1</f>
         <v>5</v>
       </c>
-      <c r="C29" s="47" t="s">
-        <v>76</v>
+      <c r="C29" s="56" t="s">
+        <v>134</v>
       </c>
-      <c r="D29" s="48" t="s">
-        <v>77</v>
+      <c r="D29" s="57" t="s">
+        <v>135</v>
       </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="52" t="s">
-        <v>78</v>
+      <c r="E29" s="58"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="61" t="s">
+        <v>136</v>
       </c>
-      <c r="I29" s="52" t="s">
-        <v>79</v>
+      <c r="I29" s="61" t="s">
+        <v>137</v>
       </c>
-      <c r="J29" s="53" t="s">
-        <v>80</v>
+      <c r="J29" s="62" t="s">
+        <v>138</v>
       </c>
-      <c r="K29" s="54"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="33"/>
-      <c r="R29" s="33"/>
-      <c r="S29" s="33"/>
-      <c r="T29" s="33"/>
-      <c r="U29" s="33"/>
-      <c r="V29" s="33"/>
-      <c r="W29" s="33"/>
-      <c r="X29" s="33"/>
-      <c r="Y29" s="33"/>
-      <c r="Z29" s="33"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="41"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="33"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="48" t="s">
-        <v>82</v>
+      <c r="A30" s="41"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="57" t="s">
+        <v>140</v>
       </c>
-      <c r="E30" s="49"/>
-      <c r="F30" s="56" t="s">
-        <v>83</v>
+      <c r="E30" s="58"/>
+      <c r="F30" s="66" t="s">
+        <v>141</v>
       </c>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="43" t="s">
-        <v>84</v>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="51" t="s">
+        <v>142</v>
       </c>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="33"/>
-      <c r="S30" s="33"/>
-      <c r="T30" s="33"/>
-      <c r="U30" s="33"/>
-      <c r="V30" s="33"/>
-      <c r="W30" s="33"/>
-      <c r="X30" s="33"/>
-      <c r="Y30" s="33"/>
-      <c r="Z30" s="33"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="41"/>
+      <c r="U30" s="41"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="41"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="41"/>
+      <c r="Z30" s="41"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="33"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="33"/>
-      <c r="S31" s="33"/>
-      <c r="T31" s="33"/>
-      <c r="U31" s="33"/>
-      <c r="V31" s="33"/>
-      <c r="W31" s="33"/>
-      <c r="X31" s="33"/>
-      <c r="Y31" s="33"/>
-      <c r="Z31" s="33"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="41"/>
+      <c r="V31" s="41"/>
+      <c r="W31" s="41"/>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="41"/>
+      <c r="Z31" s="41"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="33"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="41" t="s">
-        <v>89</v>
+      <c r="A32" s="41"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="49" t="s">
+        <v>144</v>
       </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43" t="s">
-        <v>90</v>
+      <c r="E32" s="50"/>
+      <c r="F32" s="51" t="s">
+        <v>145</v>
       </c>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="43" t="s">
-        <v>91</v>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="51" t="s">
+        <v>146</v>
       </c>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33"/>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="33"/>
-      <c r="S32" s="33"/>
-      <c r="T32" s="33"/>
-      <c r="U32" s="33"/>
-      <c r="V32" s="33"/>
-      <c r="W32" s="33"/>
-      <c r="X32" s="33"/>
-      <c r="Y32" s="33"/>
-      <c r="Z32" s="33"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
+      <c r="U32" s="41"/>
+      <c r="V32" s="41"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="41"/>
+      <c r="Z32" s="41"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="33"/>
-      <c r="B33" s="46">
+      <c r="A33" s="41"/>
+      <c r="B33" s="55">
         <f>B29+1</f>
         <v>6</v>
       </c>
-      <c r="C33" s="47" t="s">
-        <v>93</v>
+      <c r="C33" s="56" t="s">
+        <v>148</v>
       </c>
-      <c r="D33" s="48" t="s">
-        <v>94</v>
+      <c r="D33" s="57" t="s">
+        <v>149</v>
       </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="52" t="s">
-        <v>95</v>
+      <c r="E33" s="58"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="61" t="s">
+        <v>150</v>
       </c>
-      <c r="I33" s="52" t="s">
-        <v>96</v>
+      <c r="I33" s="61" t="s">
+        <v>151</v>
       </c>
-      <c r="J33" s="53" t="s">
-        <v>97</v>
+      <c r="J33" s="62" t="s">
+        <v>152</v>
       </c>
-      <c r="K33" s="54"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="33"/>
-      <c r="S33" s="33"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="33"/>
-      <c r="V33" s="33"/>
-      <c r="W33" s="33"/>
-      <c r="X33" s="33"/>
-      <c r="Y33" s="33"/>
-      <c r="Z33" s="33"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="41"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="41"/>
+      <c r="T33" s="41"/>
+      <c r="U33" s="41"/>
+      <c r="V33" s="41"/>
+      <c r="W33" s="41"/>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="41"/>
+      <c r="Z33" s="41"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="33"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="48" t="s">
-        <v>98</v>
+      <c r="A34" s="41"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="57" t="s">
+        <v>153</v>
       </c>
-      <c r="E34" s="49"/>
-      <c r="F34" s="56" t="s">
-        <v>99</v>
+      <c r="E34" s="58"/>
+      <c r="F34" s="66" t="s">
+        <v>154</v>
       </c>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="43" t="s">
-        <v>100</v>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="51" t="s">
+        <v>155</v>
       </c>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="33"/>
-      <c r="Q34" s="33"/>
-      <c r="R34" s="33"/>
-      <c r="S34" s="33"/>
-      <c r="T34" s="33"/>
-      <c r="U34" s="33"/>
-      <c r="V34" s="33"/>
-      <c r="W34" s="33"/>
-      <c r="X34" s="33"/>
-      <c r="Y34" s="33"/>
-      <c r="Z34" s="33"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="41"/>
+      <c r="R34" s="41"/>
+      <c r="S34" s="41"/>
+      <c r="T34" s="41"/>
+      <c r="U34" s="41"/>
+      <c r="V34" s="41"/>
+      <c r="W34" s="41"/>
+      <c r="X34" s="41"/>
+      <c r="Y34" s="41"/>
+      <c r="Z34" s="41"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="33"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
-      <c r="O35" s="33"/>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="33"/>
-      <c r="R35" s="33"/>
-      <c r="S35" s="33"/>
-      <c r="T35" s="33"/>
-      <c r="U35" s="33"/>
-      <c r="V35" s="33"/>
-      <c r="W35" s="33"/>
-      <c r="X35" s="33"/>
-      <c r="Y35" s="33"/>
-      <c r="Z35" s="33"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="41"/>
+      <c r="S35" s="41"/>
+      <c r="T35" s="41"/>
+      <c r="U35" s="41"/>
+      <c r="V35" s="41"/>
+      <c r="W35" s="41"/>
+      <c r="X35" s="41"/>
+      <c r="Y35" s="41"/>
+      <c r="Z35" s="41"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="33"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="41" t="s">
-        <v>113</v>
+      <c r="A36" s="41"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="49" t="s">
+        <v>157</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="43" t="s">
-        <v>114</v>
+      <c r="E36" s="50"/>
+      <c r="F36" s="51" t="s">
+        <v>158</v>
       </c>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="43" t="s">
-        <v>115</v>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="51" t="s">
+        <v>159</v>
       </c>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33"/>
-      <c r="R36" s="33"/>
-      <c r="S36" s="33"/>
-      <c r="T36" s="33"/>
-      <c r="U36" s="33"/>
-      <c r="V36" s="33"/>
-      <c r="W36" s="33"/>
-      <c r="X36" s="33"/>
-      <c r="Y36" s="33"/>
-      <c r="Z36" s="33"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="41"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
+      <c r="X36" s="41"/>
+      <c r="Y36" s="41"/>
+      <c r="Z36" s="41"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="33"/>
-      <c r="B37" s="46">
+      <c r="A37" s="41"/>
+      <c r="B37" s="55">
         <f>B33+1</f>
         <v>7</v>
       </c>
-      <c r="C37" s="47" t="s">
-        <v>117</v>
+      <c r="C37" s="56" t="s">
+        <v>161</v>
       </c>
-      <c r="D37" s="48" t="s">
-        <v>118</v>
+      <c r="D37" s="57" t="s">
+        <v>162</v>
       </c>
-      <c r="E37" s="49"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="52" t="s">
-        <v>119</v>
+      <c r="E37" s="58"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="61" t="s">
+        <v>163</v>
       </c>
-      <c r="I37" s="52" t="s">
-        <v>120</v>
+      <c r="I37" s="61" t="s">
+        <v>164</v>
       </c>
-      <c r="J37" s="53" t="s">
-        <v>121</v>
+      <c r="J37" s="62" t="s">
+        <v>165</v>
       </c>
-      <c r="K37" s="54"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
-      <c r="Q37" s="33"/>
-      <c r="R37" s="33"/>
-      <c r="S37" s="33"/>
-      <c r="T37" s="33"/>
-      <c r="U37" s="33"/>
-      <c r="V37" s="33"/>
-      <c r="W37" s="33"/>
-      <c r="X37" s="33"/>
-      <c r="Y37" s="33"/>
-      <c r="Z37" s="33"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="41"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="41"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="41"/>
+      <c r="T37" s="41"/>
+      <c r="U37" s="41"/>
+      <c r="V37" s="41"/>
+      <c r="W37" s="41"/>
+      <c r="X37" s="41"/>
+      <c r="Y37" s="41"/>
+      <c r="Z37" s="41"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="33"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="48" t="s">
-        <v>122</v>
+      <c r="A38" s="41"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="57" t="s">
+        <v>166</v>
       </c>
-      <c r="E38" s="49"/>
-      <c r="F38" s="56" t="s">
-        <v>123</v>
+      <c r="E38" s="58"/>
+      <c r="F38" s="66" t="s">
+        <v>167</v>
       </c>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="43" t="s">
-        <v>125</v>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="51" t="s">
+        <v>168</v>
       </c>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
-      <c r="Q38" s="33"/>
-      <c r="R38" s="33"/>
-      <c r="S38" s="33"/>
-      <c r="T38" s="33"/>
-      <c r="U38" s="33"/>
-      <c r="V38" s="33"/>
-      <c r="W38" s="33"/>
-      <c r="X38" s="33"/>
-      <c r="Y38" s="33"/>
-      <c r="Z38" s="33"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="41"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="41"/>
+      <c r="U38" s="41"/>
+      <c r="V38" s="41"/>
+      <c r="W38" s="41"/>
+      <c r="X38" s="41"/>
+      <c r="Y38" s="41"/>
+      <c r="Z38" s="41"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="33"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="61"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33"/>
-      <c r="Q39" s="33"/>
-      <c r="R39" s="33"/>
-      <c r="S39" s="33"/>
-      <c r="T39" s="33"/>
-      <c r="U39" s="33"/>
-      <c r="V39" s="33"/>
-      <c r="W39" s="33"/>
-      <c r="X39" s="33"/>
-      <c r="Y39" s="33"/>
-      <c r="Z39" s="33"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
+      <c r="Q39" s="41"/>
+      <c r="R39" s="41"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
+      <c r="U39" s="41"/>
+      <c r="V39" s="41"/>
+      <c r="W39" s="41"/>
+      <c r="X39" s="41"/>
+      <c r="Y39" s="41"/>
+      <c r="Z39" s="41"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="33"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="41" t="s">
-        <v>127</v>
+      <c r="A40" s="41"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="49" t="s">
+        <v>169</v>
       </c>
-      <c r="E40" s="42"/>
-      <c r="F40" s="43" t="s">
-        <v>128</v>
+      <c r="E40" s="50"/>
+      <c r="F40" s="51" t="s">
+        <v>170</v>
       </c>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="43" t="s">
-        <v>129</v>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="51" t="s">
+        <v>171</v>
       </c>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
-      <c r="R40" s="33"/>
-      <c r="S40" s="33"/>
-      <c r="T40" s="33"/>
-      <c r="U40" s="33"/>
-      <c r="V40" s="33"/>
-      <c r="W40" s="33"/>
-      <c r="X40" s="33"/>
-      <c r="Y40" s="33"/>
-      <c r="Z40" s="33"/>
+      <c r="L40" s="41"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="41"/>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="41"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="41"/>
+      <c r="T40" s="41"/>
+      <c r="U40" s="41"/>
+      <c r="V40" s="41"/>
+      <c r="W40" s="41"/>
+      <c r="X40" s="41"/>
+      <c r="Y40" s="41"/>
+      <c r="Z40" s="41"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="33"/>
-      <c r="B41" s="46">
+      <c r="A41" s="41"/>
+      <c r="B41" s="55">
         <f>B37+1</f>
         <v>8</v>
       </c>
-      <c r="C41" s="47" t="s">
-        <v>130</v>
+      <c r="C41" s="56" t="s">
+        <v>173</v>
       </c>
-      <c r="D41" s="48" t="s">
-        <v>131</v>
+      <c r="D41" s="57" t="s">
+        <v>174</v>
       </c>
-      <c r="E41" s="49"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="52" t="s">
-        <v>132</v>
+      <c r="E41" s="58"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="61" t="s">
+        <v>175</v>
       </c>
-      <c r="I41" s="52" t="s">
-        <v>133</v>
+      <c r="I41" s="61" t="s">
+        <v>176</v>
       </c>
-      <c r="J41" s="53" t="s">
-        <v>135</v>
+      <c r="J41" s="62" t="s">
+        <v>177</v>
       </c>
-      <c r="K41" s="54"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="33"/>
-      <c r="S41" s="33"/>
-      <c r="T41" s="33"/>
-      <c r="U41" s="33"/>
-      <c r="V41" s="33"/>
-      <c r="W41" s="33"/>
-      <c r="X41" s="33"/>
-      <c r="Y41" s="33"/>
-      <c r="Z41" s="33"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="41"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+      <c r="O41" s="41"/>
+      <c r="P41" s="41"/>
+      <c r="Q41" s="41"/>
+      <c r="R41" s="41"/>
+      <c r="S41" s="41"/>
+      <c r="T41" s="41"/>
+      <c r="U41" s="41"/>
+      <c r="V41" s="41"/>
+      <c r="W41" s="41"/>
+      <c r="X41" s="41"/>
+      <c r="Y41" s="41"/>
+      <c r="Z41" s="41"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="33"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="48" t="s">
-        <v>143</v>
+      <c r="A42" s="41"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="57" t="s">
+        <v>178</v>
       </c>
-      <c r="E42" s="49"/>
-      <c r="F42" s="56" t="s">
-        <v>145</v>
+      <c r="E42" s="58"/>
+      <c r="F42" s="66" t="s">
+        <v>179</v>
       </c>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="43" t="s">
-        <v>148</v>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="51" t="s">
+        <v>180</v>
       </c>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
-      <c r="O42" s="33"/>
-      <c r="P42" s="33"/>
-      <c r="Q42" s="33"/>
-      <c r="R42" s="33"/>
-      <c r="S42" s="33"/>
-      <c r="T42" s="33"/>
-      <c r="U42" s="33"/>
-      <c r="V42" s="33"/>
-      <c r="W42" s="33"/>
-      <c r="X42" s="33"/>
-      <c r="Y42" s="33"/>
-      <c r="Z42" s="33"/>
+      <c r="L42" s="41"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="41"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="41"/>
+      <c r="T42" s="41"/>
+      <c r="U42" s="41"/>
+      <c r="V42" s="41"/>
+      <c r="W42" s="41"/>
+      <c r="X42" s="41"/>
+      <c r="Y42" s="41"/>
+      <c r="Z42" s="41"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="33"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="61"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="54"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="33"/>
-      <c r="N43" s="33"/>
-      <c r="O43" s="33"/>
-      <c r="P43" s="33"/>
-      <c r="Q43" s="33"/>
-      <c r="R43" s="33"/>
-      <c r="S43" s="33"/>
-      <c r="T43" s="33"/>
-      <c r="U43" s="33"/>
-      <c r="V43" s="33"/>
-      <c r="W43" s="33"/>
-      <c r="X43" s="33"/>
-      <c r="Y43" s="33"/>
-      <c r="Z43" s="33"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="70"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="41"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="41"/>
+      <c r="O43" s="41"/>
+      <c r="P43" s="41"/>
+      <c r="Q43" s="41"/>
+      <c r="R43" s="41"/>
+      <c r="S43" s="41"/>
+      <c r="T43" s="41"/>
+      <c r="U43" s="41"/>
+      <c r="V43" s="41"/>
+      <c r="W43" s="41"/>
+      <c r="X43" s="41"/>
+      <c r="Y43" s="41"/>
+      <c r="Z43" s="41"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="1"/>

</xml_diff>